<commit_message>
adc_sample: add timing diagram
</commit_message>
<xml_diff>
--- a/embedded/adc_sample/DOC/pin分配.xlsx
+++ b/embedded/adc_sample/DOC/pin分配.xlsx
@@ -168,11 +168,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FSK控制,PWM_CH_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FSK控制,PWM_CH_4</t>
+    <t>PWM_CH_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FSK控制输出,PWM_CH_4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -549,7 +549,7 @@
   <dimension ref="A1:G13"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>

</xml_diff>

<commit_message>
adc_sample: change to use cpp framework
</commit_message>
<xml_diff>
--- a/embedded/adc_sample/DOC/pin分配.xlsx
+++ b/embedded/adc_sample/DOC/pin分配.xlsx
@@ -100,10 +100,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>雷达中频输入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PB4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -128,10 +124,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>FSK控制输出</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PA12</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -148,10 +140,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>环境光输入</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>PA8</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -164,11 +152,23 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>串口发</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>串口收</t>
+    <t>雷达中频输入ADC2_IN5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>环境光输入ADC1_IN3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FSK控制输出TIM1_CH3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>串口发uart3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>串口收uart3</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -545,7 +545,7 @@
   <dimension ref="A1:F12"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -587,7 +587,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="1" t="s">
-        <v>21</v>
+        <v>34</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
@@ -595,13 +595,13 @@
     <row r="3" spans="1:6">
       <c r="A3" s="1"/>
       <c r="B3" s="1" t="s">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="E3" s="1"/>
       <c r="F3" s="1"/>
@@ -609,7 +609,7 @@
     <row r="4" spans="1:6">
       <c r="A4" s="1"/>
       <c r="B4" s="1" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>18</v>
@@ -619,35 +619,35 @@
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:6">
       <c r="A5" s="1"/>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="6" spans="1:6">
       <c r="A6" s="1"/>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>31</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="D6" s="1" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="E6" s="1"/>
       <c r="F6" s="1"/>
@@ -655,13 +655,13 @@
     <row r="7" spans="1:6">
       <c r="A7" s="1"/>
       <c r="B7" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>8</v>
       </c>
       <c r="D7" s="1" t="s">
-        <v>28</v>
+        <v>36</v>
       </c>
       <c r="E7" s="1"/>
       <c r="F7" s="1"/>
@@ -669,7 +669,7 @@
     <row r="8" spans="1:6">
       <c r="A8" s="1"/>
       <c r="B8" s="1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>6</v>
@@ -683,7 +683,7 @@
     <row r="9" spans="1:6">
       <c r="A9" s="1"/>
       <c r="B9" s="1" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>4</v>
@@ -697,7 +697,7 @@
     <row r="10" spans="1:6">
       <c r="A10" s="1"/>
       <c r="B10" s="1" t="s">
-        <v>31</v>
+        <v>29</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>9</v>

</xml_diff>

<commit_message>
adc_sample: update pinout doc
</commit_message>
<xml_diff>
--- a/embedded/adc_sample/DOC/pin分配.xlsx
+++ b/embedded/adc_sample/DOC/pin分配.xlsx
@@ -14,11 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="40">
-  <si>
-    <t xml:space="preserve"> 序号</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="36">
   <si>
     <t>PIN</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -40,10 +36,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>DO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>AI</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -64,11 +56,95 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>PA13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA14</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SWDIO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SWCLK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DIO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>DI</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>雷达中频输入,ADC_CHANNEL_3</t>
+    <t>usart2_tx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>usart2_rx</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PB11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>雷达中频输入,ADC_CHANNEL_5</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>DIO</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPIO1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>GPIO1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RX</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SWD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SWC</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>PA10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>序号</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -76,103 +152,11 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>PA13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PA14</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SWDIO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SWCLK</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DIO</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>DI</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>usart2_tx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>usart2_rx</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC6</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>板载红色LED，低亮高灭</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC7</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>板载绿色LED，低亮高灭</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>板载蓝色LED，低亮高灭</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>板载用户按钮1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>板载用户按钮2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PB10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PB11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PC3</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PA8</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PA11</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>PWM_CH_1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>FSK控制输出,PWM_CH_4</t>
+    <t>ENRF,PWM3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>FSK,PWM4</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -234,7 +218,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -243,9 +227,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -546,10 +527,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="D5" sqref="D5"/>
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5"/>
@@ -565,206 +546,172 @@
   <sheetData>
     <row r="1" spans="1:7">
       <c r="A1" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>3</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>2</v>
-      </c>
       <c r="E1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1">
+        <v>1</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="C2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="F1" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1" t="s">
-        <v>35</v>
-      </c>
-      <c r="C2" s="1" t="s">
-        <v>7</v>
-      </c>
       <c r="D2" s="1" t="s">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="E2" s="1"/>
       <c r="F2" s="1"/>
       <c r="G2" s="1"/>
     </row>
     <row r="3" spans="1:7">
-      <c r="A3" s="1"/>
+      <c r="A3" s="1">
+        <v>2</v>
+      </c>
       <c r="B3" s="1" t="s">
-        <v>36</v>
+        <v>23</v>
       </c>
       <c r="C3" s="1" t="s">
-        <v>14</v>
+        <v>24</v>
       </c>
       <c r="D3" s="1" t="s">
-        <v>38</v>
-      </c>
-      <c r="E3" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>26</v>
+      </c>
       <c r="F3" s="1"/>
       <c r="G3" s="1"/>
     </row>
     <row r="4" spans="1:7">
-      <c r="A4" s="1"/>
+      <c r="A4" s="1">
+        <v>3</v>
+      </c>
       <c r="B4" s="1" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="C4" s="1" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D4" s="1" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="E4" s="1"/>
       <c r="F4" s="1"/>
       <c r="G4" s="1"/>
     </row>
     <row r="5" spans="1:7">
-      <c r="A5" s="1"/>
+      <c r="A5" s="1">
+        <v>4</v>
+      </c>
       <c r="B5" s="1" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="C5" s="1" t="s">
-        <v>6</v>
+        <v>33</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>24</v>
+        <v>35</v>
       </c>
       <c r="E5" s="1"/>
       <c r="F5" s="1"/>
       <c r="G5" s="1"/>
     </row>
     <row r="6" spans="1:7">
-      <c r="A6" s="1"/>
+      <c r="A6" s="1">
+        <v>5</v>
+      </c>
       <c r="B6" s="1" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
       <c r="C6" s="1" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="D6" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="E6" s="1" t="s">
         <v>27</v>
       </c>
-      <c r="E6" s="1"/>
       <c r="F6" s="1"/>
       <c r="G6" s="1"/>
     </row>
     <row r="7" spans="1:7">
-      <c r="A7" s="1"/>
+      <c r="A7" s="1">
+        <v>6</v>
+      </c>
       <c r="B7" s="1" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="C7" s="1" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="D7" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="E7" s="1"/>
       <c r="F7" s="1"/>
       <c r="G7" s="1"/>
     </row>
     <row r="8" spans="1:7">
-      <c r="A8" s="1"/>
+      <c r="A8" s="1">
+        <v>7</v>
+      </c>
       <c r="B8" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C8" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" s="1"/>
       <c r="F8" s="1"/>
       <c r="G8" s="1"/>
     </row>
     <row r="9" spans="1:7">
-      <c r="A9" s="1"/>
+      <c r="A9" s="1">
+        <v>8</v>
+      </c>
       <c r="B9" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="C9" s="1" t="s">
-        <v>12</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="E9" s="1"/>
       <c r="F9" s="1"/>
       <c r="G9" s="1"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="A10" s="1"/>
-      <c r="B10" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C10" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="E10" s="1"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="1"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="A11" s="1"/>
-      <c r="B11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="C11" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="D11" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="E11" s="1"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="1"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="A12" s="1"/>
-      <c r="B12" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="D12" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="E12" s="1"/>
-      <c r="F12" s="1"/>
-      <c r="G12" s="1"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="D13" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="1"/>
-      <c r="F13" s="1"/>
-      <c r="G13" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>